<commit_message>
Cronograma por semana de ejemplo de tallado
</commit_message>
<xml_diff>
--- a/Planificación del proyecto/Cronograma Equipo 01 v2.xlsx
+++ b/Planificación del proyecto/Cronograma Equipo 01 v2.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeDicenTecno\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Licenciatura en Sistemas\3º AÑO\2º Cuatrimestre\Proyecto de Software\TP cuatrimesatral\Ecommerce-Sports\Planificación del proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE67149-5381-4B7B-9014-BBAD2EB462FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="28800" windowHeight="11085" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CC" sheetId="1" r:id="rId1"/>
     <sheet name="CI1" sheetId="2" r:id="rId2"/>
     <sheet name="CI2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -758,7 +759,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
@@ -983,7 +984,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1096,12 +1097,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1109,25 +1104,37 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1342,7 +1349,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1359,20 +1366,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="53" t="s">
+      <c r="C1" s="52"/>
+      <c r="D1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="51" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1410,16 +1417,16 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="54"/>
+      <c r="A2" s="52"/>
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
       <c r="G2" s="2">
         <f t="shared" ref="G2:H2" si="0">H2-7</f>
         <v>44067</v>
@@ -4836,7 +4843,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -4855,91 +4862,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="58" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="58" t="s">
+      <c r="H1" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="58" t="s">
+      <c r="I1" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="58" t="s">
+      <c r="J1" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="55" t="s">
+      <c r="K1" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="56"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="61" t="s">
+      <c r="L1" s="61"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="56"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="55" t="s">
+      <c r="O1" s="61"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="56"/>
-      <c r="S1" s="57"/>
-      <c r="T1" s="61" t="s">
+      <c r="R1" s="61"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="56"/>
-      <c r="V1" s="57"/>
-      <c r="W1" s="55" t="s">
+      <c r="U1" s="61"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="57"/>
-      <c r="Z1" s="61" t="s">
+      <c r="X1" s="61"/>
+      <c r="Y1" s="62"/>
+      <c r="Z1" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="57"/>
-      <c r="AC1" s="55" t="s">
+      <c r="AA1" s="61"/>
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="57"/>
-      <c r="AF1" s="61" t="s">
+      <c r="AD1" s="61"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="56"/>
-      <c r="AH1" s="57"/>
-      <c r="AI1" s="55" t="s">
+      <c r="AG1" s="61"/>
+      <c r="AH1" s="62"/>
+      <c r="AI1" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="56"/>
-      <c r="AK1" s="57"/>
+      <c r="AJ1" s="61"/>
+      <c r="AK1" s="62"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A2" s="59"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
       <c r="K2" s="3">
         <v>44081</v>
       </c>
@@ -5022,20 +5029,20 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A3" s="60"/>
+      <c r="A3" s="55"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
       <c r="K3" s="9" t="s">
         <v>36</v>
       </c>
@@ -35061,16 +35068,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="J1:J3"/>
@@ -35079,6 +35076,16 @@
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -35086,11 +35093,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AK43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -35104,91 +35111,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="58" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="58" t="s">
+      <c r="H1" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="58" t="s">
+      <c r="I1" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="58" t="s">
+      <c r="J1" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="55" t="s">
+      <c r="K1" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="56"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="61" t="s">
+      <c r="L1" s="61"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="56"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="55" t="s">
+      <c r="O1" s="61"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="56"/>
-      <c r="S1" s="57"/>
-      <c r="T1" s="61" t="s">
+      <c r="R1" s="61"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="56"/>
-      <c r="V1" s="57"/>
-      <c r="W1" s="55" t="s">
+      <c r="U1" s="61"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="57"/>
-      <c r="Z1" s="61" t="s">
+      <c r="X1" s="61"/>
+      <c r="Y1" s="62"/>
+      <c r="Z1" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="57"/>
-      <c r="AC1" s="55" t="s">
+      <c r="AA1" s="61"/>
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="57"/>
-      <c r="AF1" s="61" t="s">
+      <c r="AD1" s="61"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="56"/>
-      <c r="AH1" s="57"/>
-      <c r="AI1" s="55" t="s">
+      <c r="AG1" s="61"/>
+      <c r="AH1" s="62"/>
+      <c r="AI1" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="56"/>
-      <c r="AK1" s="57"/>
+      <c r="AJ1" s="61"/>
+      <c r="AK1" s="62"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A2" s="59"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
       <c r="K2" s="3">
         <v>44081</v>
       </c>
@@ -35271,20 +35278,20 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A3" s="60"/>
+      <c r="A3" s="55"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
       <c r="K3" s="9" t="s">
         <v>36</v>
       </c>
@@ -35395,7 +35402,7 @@
         <v>44088</v>
       </c>
       <c r="J4" s="49"/>
-      <c r="K4" s="52" t="s">
+      <c r="K4" s="50" t="s">
         <v>201</v>
       </c>
       <c r="L4" s="48"/>
@@ -36470,15 +36477,15 @@
       <c r="B24" s="46" t="s">
         <v>242</v>
       </c>
-      <c r="C24" s="46" t="s">
+      <c r="C24" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="41"/>
-      <c r="E24" s="46" t="s">
+      <c r="D24" s="65"/>
+      <c r="E24" s="64" t="s">
         <v>186</v>
       </c>
-      <c r="F24" s="41"/>
-      <c r="G24" s="46" t="s">
+      <c r="F24" s="65"/>
+      <c r="G24" s="64" t="s">
         <v>185</v>
       </c>
       <c r="H24" s="25"/>
@@ -36523,15 +36530,15 @@
       <c r="B25" s="41" t="s">
         <v>206</v>
       </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="46" t="s">
+      <c r="C25" s="65"/>
+      <c r="D25" s="64" t="s">
         <v>177</v>
       </c>
-      <c r="E25" s="46" t="s">
+      <c r="E25" s="64" t="s">
         <v>182</v>
       </c>
-      <c r="F25" s="41"/>
-      <c r="G25" s="46" t="s">
+      <c r="F25" s="65"/>
+      <c r="G25" s="64" t="s">
         <v>179</v>
       </c>
       <c r="H25" s="20">
@@ -36580,15 +36587,15 @@
         <v>23</v>
       </c>
       <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="46" t="s">
+      <c r="C26" s="65"/>
+      <c r="D26" s="64" t="s">
         <v>178</v>
       </c>
-      <c r="E26" s="46" t="s">
+      <c r="E26" s="64" t="s">
         <v>183</v>
       </c>
-      <c r="F26" s="41"/>
-      <c r="G26" s="46" t="s">
+      <c r="F26" s="65"/>
+      <c r="G26" s="64" t="s">
         <v>179</v>
       </c>
       <c r="H26" s="20">
@@ -36639,17 +36646,17 @@
       <c r="B27" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="65" t="s">
         <v>207</v>
       </c>
-      <c r="D27" s="41" t="s">
+      <c r="D27" s="65" t="s">
         <v>208</v>
       </c>
-      <c r="E27" s="41" t="s">
+      <c r="E27" s="65" t="s">
         <v>209</v>
       </c>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41" t="s">
+      <c r="F27" s="65"/>
+      <c r="G27" s="65" t="s">
         <v>185</v>
       </c>
       <c r="H27" s="20">
@@ -36700,17 +36707,17 @@
       <c r="B28" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="41" t="s">
+      <c r="C28" s="65" t="s">
         <v>210</v>
       </c>
-      <c r="D28" s="41" t="s">
+      <c r="D28" s="65" t="s">
         <v>210</v>
       </c>
-      <c r="E28" s="41" t="s">
+      <c r="E28" s="65" t="s">
         <v>182</v>
       </c>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41" t="s">
+      <c r="F28" s="65"/>
+      <c r="G28" s="65" t="s">
         <v>179</v>
       </c>
       <c r="H28" s="20">
@@ -36761,15 +36768,15 @@
       <c r="B29" s="41" t="s">
         <v>212</v>
       </c>
-      <c r="C29" s="41" t="s">
+      <c r="C29" s="65" t="s">
         <v>213</v>
       </c>
-      <c r="D29" s="41"/>
-      <c r="E29" s="46" t="s">
+      <c r="D29" s="65"/>
+      <c r="E29" s="64" t="s">
         <v>183</v>
       </c>
-      <c r="F29" s="41"/>
-      <c r="G29" s="46" t="s">
+      <c r="F29" s="65"/>
+      <c r="G29" s="64" t="s">
         <v>230</v>
       </c>
       <c r="H29" s="20">
@@ -36814,15 +36821,15 @@
         <v>25</v>
       </c>
       <c r="B30" s="47"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="51" t="s">
+      <c r="C30" s="66"/>
+      <c r="D30" s="67" t="s">
         <v>219</v>
       </c>
-      <c r="E30" s="46" t="s">
+      <c r="E30" s="64" t="s">
         <v>183</v>
       </c>
-      <c r="F30" s="41"/>
-      <c r="G30" s="51" t="s">
+      <c r="F30" s="65"/>
+      <c r="G30" s="67" t="s">
         <v>179</v>
       </c>
       <c r="H30" s="20">
@@ -36867,15 +36874,15 @@
         <v>26</v>
       </c>
       <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41" t="s">
+      <c r="C31" s="65"/>
+      <c r="D31" s="65" t="s">
         <v>220</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="64" t="s">
         <v>183</v>
       </c>
-      <c r="F31" s="41"/>
-      <c r="G31" s="51" t="s">
+      <c r="F31" s="65"/>
+      <c r="G31" s="67" t="s">
         <v>179</v>
       </c>
       <c r="H31" s="20">
@@ -36920,15 +36927,15 @@
         <v>27</v>
       </c>
       <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="51" t="s">
+      <c r="C32" s="65"/>
+      <c r="D32" s="67" t="s">
         <v>214</v>
       </c>
-      <c r="E32" s="46" t="s">
+      <c r="E32" s="64" t="s">
         <v>183</v>
       </c>
-      <c r="F32" s="41"/>
-      <c r="G32" s="51" t="s">
+      <c r="F32" s="65"/>
+      <c r="G32" s="67" t="s">
         <v>179</v>
       </c>
       <c r="H32" s="20">
@@ -36975,13 +36982,13 @@
       <c r="B33" s="41" t="s">
         <v>215</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="41"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="46" t="s">
+      <c r="D33" s="65"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="64" t="s">
         <v>237</v>
       </c>
       <c r="H33" s="20">
@@ -37026,15 +37033,15 @@
         <v>29</v>
       </c>
       <c r="B34" s="47"/>
-      <c r="C34" s="50"/>
-      <c r="D34" s="41" t="s">
+      <c r="C34" s="66"/>
+      <c r="D34" s="65" t="s">
         <v>221</v>
       </c>
-      <c r="E34" s="41" t="s">
+      <c r="E34" s="65" t="s">
         <v>228</v>
       </c>
-      <c r="F34" s="41"/>
-      <c r="G34" s="41" t="s">
+      <c r="F34" s="65"/>
+      <c r="G34" s="65" t="s">
         <v>235</v>
       </c>
       <c r="H34" s="20">
@@ -37079,15 +37086,15 @@
         <v>30</v>
       </c>
       <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41" t="s">
+      <c r="C35" s="65"/>
+      <c r="D35" s="65" t="s">
         <v>222</v>
       </c>
-      <c r="E35" s="41" t="s">
+      <c r="E35" s="65" t="s">
         <v>209</v>
       </c>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41" t="s">
+      <c r="F35" s="65"/>
+      <c r="G35" s="65" t="s">
         <v>236</v>
       </c>
       <c r="H35" s="20">
@@ -37132,15 +37139,15 @@
         <v>31</v>
       </c>
       <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41" t="s">
+      <c r="C36" s="65"/>
+      <c r="D36" s="65" t="s">
         <v>223</v>
       </c>
-      <c r="E36" s="41" t="s">
+      <c r="E36" s="65" t="s">
         <v>229</v>
       </c>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41" t="s">
+      <c r="F36" s="65"/>
+      <c r="G36" s="65" t="s">
         <v>233</v>
       </c>
       <c r="H36" s="20">
@@ -37185,15 +37192,15 @@
         <v>32</v>
       </c>
       <c r="B37" s="41"/>
-      <c r="C37" s="41" t="s">
+      <c r="C37" s="65" t="s">
         <v>231</v>
       </c>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41" t="s">
+      <c r="D37" s="65"/>
+      <c r="E37" s="65" t="s">
         <v>243</v>
       </c>
-      <c r="F37" s="41"/>
-      <c r="G37" s="41" t="s">
+      <c r="F37" s="65"/>
+      <c r="G37" s="65" t="s">
         <v>240</v>
       </c>
       <c r="H37" s="43">
@@ -37240,15 +37247,15 @@
       <c r="B38" s="41" t="s">
         <v>225</v>
       </c>
-      <c r="C38" s="41" t="s">
+      <c r="C38" s="65" t="s">
         <v>216</v>
       </c>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41" t="s">
+      <c r="D38" s="65"/>
+      <c r="E38" s="65" t="s">
         <v>243</v>
       </c>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41" t="s">
+      <c r="F38" s="65"/>
+      <c r="G38" s="65" t="s">
         <v>236</v>
       </c>
       <c r="H38" s="43">
@@ -37293,15 +37300,15 @@
         <v>34</v>
       </c>
       <c r="B39" s="41"/>
-      <c r="C39" s="41"/>
-      <c r="D39" s="41" t="s">
+      <c r="C39" s="65"/>
+      <c r="D39" s="65" t="s">
         <v>239</v>
       </c>
-      <c r="E39" s="41" t="s">
+      <c r="E39" s="65" t="s">
         <v>243</v>
       </c>
-      <c r="F39" s="41"/>
-      <c r="G39" s="41" t="s">
+      <c r="F39" s="65"/>
+      <c r="G39" s="65" t="s">
         <v>233</v>
       </c>
       <c r="H39" s="43">
@@ -37346,15 +37353,15 @@
         <v>34</v>
       </c>
       <c r="B40" s="41"/>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41" t="s">
+      <c r="C40" s="65"/>
+      <c r="D40" s="65" t="s">
         <v>224</v>
       </c>
-      <c r="E40" s="41" t="s">
+      <c r="E40" s="65" t="s">
         <v>209</v>
       </c>
-      <c r="F40" s="41"/>
-      <c r="G40" s="41" t="s">
+      <c r="F40" s="65"/>
+      <c r="G40" s="65" t="s">
         <v>233</v>
       </c>
       <c r="H40" s="43">
@@ -37401,13 +37408,13 @@
       <c r="B41" s="41" t="s">
         <v>226</v>
       </c>
-      <c r="C41" s="41" t="s">
+      <c r="C41" s="65" t="s">
         <v>217</v>
       </c>
-      <c r="D41" s="41"/>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="41"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="65"/>
+      <c r="F41" s="65"/>
+      <c r="G41" s="65"/>
       <c r="H41" s="43"/>
       <c r="I41" s="43"/>
       <c r="J41" s="41"/>
@@ -37444,15 +37451,15 @@
         <v>36</v>
       </c>
       <c r="B42" s="41"/>
-      <c r="C42" s="41"/>
-      <c r="D42" s="41" t="s">
+      <c r="C42" s="65"/>
+      <c r="D42" s="65" t="s">
         <v>218</v>
       </c>
-      <c r="E42" s="41" t="s">
+      <c r="E42" s="65" t="s">
         <v>182</v>
       </c>
-      <c r="F42" s="41"/>
-      <c r="G42" s="41" t="s">
+      <c r="F42" s="65"/>
+      <c r="G42" s="65" t="s">
         <v>236</v>
       </c>
       <c r="H42" s="43">
@@ -37497,15 +37504,15 @@
         <v>37</v>
       </c>
       <c r="B43" s="41"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41" t="s">
+      <c r="C43" s="65"/>
+      <c r="D43" s="65" t="s">
         <v>227</v>
       </c>
-      <c r="E43" s="41" t="s">
+      <c r="E43" s="65" t="s">
         <v>182</v>
       </c>
-      <c r="F43" s="41"/>
-      <c r="G43" s="41" t="s">
+      <c r="F43" s="65"/>
+      <c r="G43" s="65" t="s">
         <v>233</v>
       </c>
       <c r="H43" s="43">
@@ -37547,12 +37554,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I1:I3"/>
@@ -37565,6 +37566,12 @@
     <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>